<commit_message>
[ issue #8 ] First draft of DC pipeline (IMP: with debugging that needs to be removed before integrating to master!)
</commit_message>
<xml_diff>
--- a/aliada/src/site/analysis/mapping_dctordf_v1.1.xlsx
+++ b/aliada/src/site/analysis/mapping_dctordf_v1.1.xlsx
@@ -20,33 +20,6 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="E13" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b val="true"/>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">Autor:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">URI should be identifier
-</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="G75" authorId="0">
       <text>
         <r>
@@ -872,7 +845,7 @@
     <t>poster</t>
   </si>
   <si>
-    <t>Portfolio titulo original   </t>
+    <t>Portfolio titulo original</t>
   </si>
   <si>
     <t>image</t>
@@ -884,57 +857,83 @@
     <t>alternative</t>
   </si>
   <si>
-    <t>Title                       </t>
-  </si>
-  <si>
-    <t>Portfolio actors            </t>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Portfolio actors</t>
   </si>
   <si>
     <t>dc:contributor</t>
   </si>
   <si>
-    <t>Portfolio director          </t>
-  </si>
-  <si>
-    <t>Portfolio fecha             </t>
-  </si>
-  <si>
-    <t>Portfolio fecha Vitoria     </t>
-  </si>
-  <si>
-    <t>Portfolio teatro            </t>
+    <t>Portfolio director</t>
+  </si>
+  <si>
+    <t>Portfolio fecha</t>
+  </si>
+  <si>
+    <t>Portfolio fecha Vitoria</t>
+  </si>
+  <si>
+    <t>Portfolio teatro</t>
   </si>
   <si>
     <t>dc:coverage</t>
   </si>
   <si>
-    <t>Portfolio cartel peli       </t>
-  </si>
-  <si>
-    <t>Genero portfolio            </t>
+    <t>Portfolio cartel peli</t>
+  </si>
+  <si>
+    <t>Genero portfolio</t>
   </si>
   <si>
     <t>dc:subject</t>
   </si>
   <si>
-    <t>Portfolio signature         </t>
+    <t>Portfolio signature</t>
   </si>
   <si>
     <t>dc:identifier</t>
   </si>
   <si>
-    <t>Portfolio notas             </t>
-  </si>
-  <si>
-    <t>Portfolio contraportada     </t>
-  </si>
-  <si>
-    <t>Portfolio trailer youtube   </t>
+    <t>Portfolio notas</t>
+  </si>
+  <si>
+    <t>Portfolio contraportada</t>
+  </si>
+  <si>
+    <t>Portfolio trailer youtube</t>
   </si>
   <si>
     <t>http://catalogo.artium.org/ana-karenina-i</t>
   </si>
   <si>
+    <r>
+      <t xml:space="preserve">E33 Linguistic Object or E73 Information Object </t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">P129 is about (is subject of):</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Ε1 CRM Entity</t>
+    </r>
+  </si>
+  <si>
     <t>Programas de cine: http://catalogo.artium.org/programasdecine</t>
   </si>
   <si>
@@ -944,61 +943,58 @@
     <t>dossier</t>
   </si>
   <si>
-    <t>Title               </t>
-  </si>
-  <si>
     <t>text</t>
   </si>
   <si>
-    <t>Body                </t>
-  </si>
-  <si>
-    <t>Ordenacion          </t>
-  </si>
-  <si>
-    <t>Exposiciones        </t>
+    <t>Body</t>
+  </si>
+  <si>
+    <t>Ordenacion</t>
+  </si>
+  <si>
+    <t>Exposiciones</t>
   </si>
   <si>
     <t>dc: relation</t>
   </si>
   <si>
-    <t>Exposiciones fecha  </t>
-  </si>
-  <si>
-    <t>Letras              </t>
-  </si>
-  <si>
-    <t>Artista             </t>
-  </si>
-  <si>
-    <t>Artistas            </t>
-  </si>
-  <si>
-    <t>Director            </t>
-  </si>
-  <si>
-    <t>Actores             </t>
-  </si>
-  <si>
-    <t>Pelicula            </t>
-  </si>
-  <si>
-    <t>Peliculas           </t>
-  </si>
-  <si>
-    <t>Global presencion   </t>
-  </si>
-  <si>
-    <t>Global imagen       </t>
+    <t>Exposiciones fecha</t>
+  </si>
+  <si>
+    <t>Letras</t>
+  </si>
+  <si>
+    <t>Artista</t>
+  </si>
+  <si>
+    <t>Artistas</t>
+  </si>
+  <si>
+    <t>Director</t>
+  </si>
+  <si>
+    <t>Actores</t>
+  </si>
+  <si>
+    <t>Pelicula</t>
+  </si>
+  <si>
+    <t>Peliculas</t>
+  </si>
+  <si>
+    <t>Global presencion</t>
+  </si>
+  <si>
+    <t>Global imagen</t>
   </si>
   <si>
     <t>Book imagen cabecera</t>
   </si>
   <si>
-    <t>Images              </t>
-  </si>
-  <si>
-    <t>Tipo                </t>
+    <t>Images</t>
+  </si>
+  <si>
+    <t>Tipo</t>
   </si>
   <si>
     <t>dc:format</t>
@@ -1197,7 +1193,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1262,16 +1258,24 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="11" fillId="4" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -1280,6 +1284,10 @@
     </xf>
     <xf numFmtId="164" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1363,7 +1371,7 @@
   <dimension ref="A1:L75"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="11:11"/>
+      <selection pane="topLeft" activeCell="I18" activeCellId="0" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1503,7 +1511,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" s="10" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="10" t="s">
         <v>21</v>
       </c>
@@ -1519,12 +1527,16 @@
       <c r="E7" s="10" t="s">
         <v>29</v>
       </c>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
       <c r="H7" s="10" t="s">
         <v>26</v>
       </c>
       <c r="I7" s="11" t="s">
         <v>30</v>
       </c>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
       <c r="L7" s="12" t="n">
         <v>245</v>
       </c>
@@ -1662,6 +1674,7 @@
       <c r="I12" s="3" t="s">
         <v>47</v>
       </c>
+      <c r="L12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
@@ -1687,85 +1700,90 @@
       <c r="I13" s="3" t="s">
         <v>50</v>
       </c>
+      <c r="L13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="0" t="s">
+      <c r="C14" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="E14" s="0" t="s">
+      <c r="E14" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="G14" s="16" t="s">
+      <c r="F14" s="16"/>
+      <c r="G14" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="H14" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="I14" s="3" t="s">
+      <c r="I14" s="11" t="s">
         <v>54</v>
       </c>
+      <c r="L14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="0" t="s">
+      <c r="C15" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="E15" s="0" t="s">
+      <c r="E15" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="G15" s="16" t="s">
+      <c r="F15" s="16"/>
+      <c r="G15" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="H15" s="2" t="s">
+      <c r="H15" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="I15" s="3" t="s">
+      <c r="I15" s="11" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="L15" s="0"/>
+    </row>
+    <row r="16" s="16" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="B16" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="0" t="s">
+      <c r="C16" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D16" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="E16" s="0" t="s">
+      <c r="E16" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="F16" s="0" t="s">
+      <c r="F16" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="G16" s="17" t="s">
+      <c r="G16" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="H16" s="2" t="s">
+      <c r="H16" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="I16" s="3" t="s">
+      <c r="I16" s="11" t="s">
         <v>60</v>
       </c>
     </row>
@@ -1792,8 +1810,9 @@
       <c r="I17" s="3" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="L17" s="0"/>
+    </row>
+    <row r="18" customFormat="false" ht="43.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
         <v>21</v>
       </c>
@@ -1819,8 +1838,9 @@
       <c r="I18" s="3" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="L18" s="0"/>
+    </row>
+    <row r="19" customFormat="false" ht="38.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
         <v>21</v>
       </c>
@@ -1833,7 +1853,7 @@
       <c r="D19" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E19" s="18" t="s">
+      <c r="E19" s="19" t="s">
         <v>64</v>
       </c>
       <c r="G19" s="0"/>
@@ -1843,6 +1863,7 @@
       <c r="I19" s="3" t="s">
         <v>65</v>
       </c>
+      <c r="L19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
@@ -1863,7 +1884,7 @@
       <c r="F20" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="G20" s="16" t="s">
+      <c r="G20" s="20" t="s">
         <v>22</v>
       </c>
       <c r="H20" s="2" t="s">
@@ -1872,6 +1893,7 @@
       <c r="I20" s="3" t="s">
         <v>68</v>
       </c>
+      <c r="L20" s="0"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
@@ -1899,6 +1921,7 @@
       <c r="I21" s="3" t="s">
         <v>70</v>
       </c>
+      <c r="L21" s="0"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
@@ -1916,49 +1939,52 @@
       <c r="E22" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="G22" s="16" t="s">
+      <c r="G22" s="20" t="s">
         <v>24</v>
       </c>
       <c r="H22" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="I22" s="19" t="s">
+      <c r="I22" s="21" t="s">
         <v>71</v>
       </c>
+      <c r="L22" s="0"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+      <c r="A23" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="0" t="s">
+      <c r="B23" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C23" s="0" t="s">
+      <c r="C23" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="D23" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="E23" s="0" t="s">
+      <c r="E23" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="F23" s="0" t="s">
+      <c r="F23" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="G23" s="16" t="s">
+      <c r="G23" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="H23" s="2" t="s">
+      <c r="H23" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="I23" s="3" t="s">
+      <c r="I23" s="11" t="s">
         <v>75</v>
       </c>
+      <c r="L23" s="0"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="G24" s="0"/>
       <c r="H24" s="0"/>
       <c r="I24" s="0"/>
+      <c r="L24" s="0"/>
     </row>
     <row r="25" s="10" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="10" t="s">
@@ -1973,7 +1999,7 @@
       <c r="D25" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="E25" s="20" t="s">
+      <c r="E25" s="22" t="s">
         <v>80</v>
       </c>
       <c r="F25" s="10" t="s">
@@ -1981,7 +2007,7 @@
       </c>
       <c r="L25" s="12"/>
     </row>
-    <row r="26" s="10" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="10" t="s">
         <v>76</v>
       </c>
@@ -1994,9 +2020,10 @@
       <c r="D26" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="E26" s="20" t="s">
+      <c r="E26" s="22" t="s">
         <v>80</v>
       </c>
+      <c r="G26" s="10"/>
       <c r="H26" s="10" t="s">
         <v>26</v>
       </c>
@@ -2085,25 +2112,24 @@
       <c r="H30" s="0"/>
       <c r="I30" s="0"/>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
+    <row r="31" s="10" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A31" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="B31" s="0" t="s">
+      <c r="B31" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="C31" s="0" t="s">
+      <c r="C31" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="D31" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="E31" s="15" t="s">
+      <c r="E31" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="G31" s="0"/>
-      <c r="H31" s="0"/>
-      <c r="I31" s="0"/>
+      <c r="F31" s="16"/>
+      <c r="L31" s="12"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
@@ -2138,7 +2164,7 @@
       <c r="D33" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E33" s="18" t="s">
+      <c r="E33" s="19" t="s">
         <v>92</v>
       </c>
       <c r="G33" s="0"/>
@@ -2178,7 +2204,7 @@
       <c r="D35" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="E35" s="18" t="s">
+      <c r="E35" s="19" t="s">
         <v>32</v>
       </c>
       <c r="G35" s="0"/>
@@ -2226,83 +2252,85 @@
       <c r="I37" s="0"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
+      <c r="A38" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="B38" s="0" t="s">
+      <c r="B38" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="C38" s="0" t="s">
+      <c r="C38" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="D38" s="1" t="s">
+      <c r="D38" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="E38" s="0" t="s">
+      <c r="E38" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="G38" s="16" t="s">
+      <c r="F38" s="16"/>
+      <c r="G38" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="H38" s="2" t="s">
+      <c r="H38" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="I38" s="3" t="s">
+      <c r="I38" s="11" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
+      <c r="A39" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="B39" s="0" t="s">
+      <c r="B39" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="C39" s="0" t="s">
+      <c r="C39" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="D39" s="1" t="s">
+      <c r="D39" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="E39" s="0" t="s">
+      <c r="E39" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="G39" s="16" t="s">
+      <c r="F39" s="16"/>
+      <c r="G39" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="H39" s="2" t="s">
+      <c r="H39" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="I39" s="3" t="s">
+      <c r="I39" s="11" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
+      <c r="A40" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="B40" s="0" t="s">
+      <c r="B40" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="C40" s="0" t="s">
+      <c r="C40" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="D40" s="1" t="s">
+      <c r="D40" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="E40" s="0" t="s">
+      <c r="E40" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="F40" s="0" t="s">
+      <c r="F40" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="G40" s="17" t="s">
+      <c r="G40" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="H40" s="2" t="s">
+      <c r="H40" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="I40" s="3" t="s">
+      <c r="I40" s="11" t="s">
         <v>60</v>
       </c>
     </row>
@@ -2357,29 +2385,30 @@
         <v>63</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
+    <row r="43" s="10" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A43" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="B43" s="0" t="s">
+      <c r="B43" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="C43" s="0" t="s">
+      <c r="C43" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="D43" s="1" t="s">
+      <c r="D43" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="E43" s="18" t="s">
+      <c r="E43" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="G43" s="0"/>
-      <c r="H43" s="2" t="s">
+      <c r="F43" s="16"/>
+      <c r="H43" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="I43" s="3" t="s">
-        <v>65</v>
-      </c>
+      <c r="I43" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="L43" s="12"/>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
@@ -2400,7 +2429,7 @@
       <c r="F44" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="G44" s="16" t="s">
+      <c r="G44" s="20" t="s">
         <v>79</v>
       </c>
       <c r="H44" s="2" t="s">
@@ -2453,42 +2482,42 @@
       <c r="E46" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="G46" s="16" t="s">
+      <c r="G46" s="20" t="s">
         <v>79</v>
       </c>
       <c r="H46" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="I46" s="19" t="s">
+      <c r="I46" s="21" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="s">
+      <c r="A47" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="B47" s="0" t="s">
+      <c r="B47" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="C47" s="0" t="s">
+      <c r="C47" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="D47" s="1" t="s">
+      <c r="D47" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="E47" s="0" t="s">
+      <c r="E47" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="F47" s="0" t="s">
+      <c r="F47" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="G47" s="16" t="s">
-        <v>99</v>
-      </c>
-      <c r="H47" s="2" t="s">
+      <c r="G47" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="H47" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="I47" s="3" t="s">
+      <c r="I47" s="11" t="s">
         <v>75</v>
       </c>
     </row>
@@ -2498,35 +2527,36 @@
       <c r="I48" s="0"/>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="B49" s="0" t="s">
+      <c r="A49" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="C49" s="0" t="s">
+      <c r="B49" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="D49" s="1" t="s">
+      <c r="C49" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="D49" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="E49" s="0" t="s">
+      <c r="E49" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="G49" s="0"/>
-      <c r="H49" s="2" t="s">
+      <c r="F49" s="16"/>
+      <c r="G49" s="10"/>
+      <c r="H49" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="I49" s="3" t="s">
+      <c r="I49" s="11" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C50" s="0" t="s">
         <v>104</v>
@@ -2543,10 +2573,10 @@
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C51" s="0" t="s">
         <v>105</v>
@@ -2563,10 +2593,10 @@
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C52" s="0" t="s">
         <v>106</v>
@@ -2583,10 +2613,10 @@
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C53" s="0" t="s">
         <v>108</v>
@@ -2603,10 +2633,10 @@
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C54" s="0" t="s">
         <v>109</v>
@@ -2623,10 +2653,10 @@
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C55" s="0" t="s">
         <v>110</v>
@@ -2643,10 +2673,10 @@
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C56" s="0" t="s">
         <v>111</v>
@@ -2663,10 +2693,10 @@
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C57" s="0" t="s">
         <v>112</v>
@@ -2683,10 +2713,10 @@
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C58" s="0" t="s">
         <v>113</v>
@@ -2703,10 +2733,10 @@
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C59" s="0" t="s">
         <v>114</v>
@@ -2723,10 +2753,10 @@
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C60" s="0" t="s">
         <v>115</v>
@@ -2743,10 +2773,10 @@
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C61" s="0" t="s">
         <v>116</v>
@@ -2763,10 +2793,10 @@
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C62" s="0" t="s">
         <v>117</v>
@@ -2783,10 +2813,10 @@
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C63" s="0" t="s">
         <v>118</v>
@@ -2803,10 +2833,10 @@
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C64" s="0" t="s">
         <v>119</v>
@@ -2823,10 +2853,10 @@
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C65" s="0" t="s">
         <v>120</v>
@@ -2843,10 +2873,10 @@
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C66" s="0" t="s">
         <v>51</v>
@@ -2857,7 +2887,7 @@
       <c r="E66" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="G66" s="16" t="s">
+      <c r="G66" s="20" t="s">
         <v>53</v>
       </c>
       <c r="H66" s="2" t="s">
@@ -2869,10 +2899,10 @@
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C67" s="0" t="s">
         <v>51</v>
@@ -2883,7 +2913,7 @@
       <c r="E67" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="G67" s="16" t="s">
+      <c r="G67" s="20" t="s">
         <v>56</v>
       </c>
       <c r="H67" s="2" t="s">
@@ -2895,10 +2925,10 @@
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C68" s="0" t="s">
         <v>51</v>
@@ -2912,7 +2942,7 @@
       <c r="F68" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="G68" s="17" t="s">
+      <c r="G68" s="23" t="s">
         <v>122</v>
       </c>
       <c r="H68" s="2" t="s">
@@ -2924,10 +2954,10 @@
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C69" s="0" t="s">
         <v>51</v>
@@ -2948,10 +2978,10 @@
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C70" s="0" t="s">
         <v>51</v>
@@ -2973,36 +3003,37 @@
         <v>63</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A71" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="B71" s="0" t="s">
+    <row r="71" s="10" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A71" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="C71" s="0" t="s">
+      <c r="B71" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="C71" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="D71" s="1" t="s">
+      <c r="D71" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="E71" s="18" t="s">
+      <c r="E71" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="G71" s="0"/>
-      <c r="H71" s="2" t="s">
+      <c r="F71" s="16"/>
+      <c r="H71" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="I71" s="3" t="s">
-        <v>65</v>
-      </c>
+      <c r="I71" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="L71" s="12"/>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C72" s="0" t="s">
         <v>51</v>
@@ -3016,7 +3047,7 @@
       <c r="F72" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="G72" s="16" t="s">
+      <c r="G72" s="20" t="s">
         <v>103</v>
       </c>
       <c r="H72" s="2" t="s">
@@ -3028,10 +3059,10 @@
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C73" s="0" t="s">
         <v>51</v>
@@ -3055,10 +3086,10 @@
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C74" s="0" t="s">
         <v>51</v>
@@ -3069,22 +3100,22 @@
       <c r="E74" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="G74" s="16" t="s">
+      <c r="G74" s="20" t="s">
         <v>103</v>
       </c>
       <c r="H74" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="I74" s="19" t="s">
+      <c r="I74" s="21" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C75" s="0" t="s">
         <v>51</v>
@@ -3098,8 +3129,8 @@
       <c r="F75" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="G75" s="19" t="s">
-        <v>100</v>
+      <c r="G75" s="21" t="s">
+        <v>101</v>
       </c>
       <c r="H75" s="2" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
[ issue #8 ] Additional DC mappings + example of a DC (small) dataset
</commit_message>
<xml_diff>
--- a/aliada/src/site/analysis/mapping_dctordf_v1.1.xlsx
+++ b/aliada/src/site/analysis/mapping_dctordf_v1.1.xlsx
@@ -1246,7 +1246,11 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1258,10 +1262,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1270,7 +1270,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1282,12 +1282,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1370,8 +1370,8 @@
   </sheetPr>
   <dimension ref="A1:L75"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I18" activeCellId="0" sqref="I18"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I21" activeCellId="0" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1541,85 +1541,85 @@
         <v>245</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="61.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+    <row r="8" s="13" customFormat="true" ht="61.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="0" t="s">
+      <c r="E8" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="G8" s="0"/>
-      <c r="H8" s="2" t="s">
+      <c r="G8" s="10"/>
+      <c r="H8" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="I8" s="3" t="s">
+      <c r="I8" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="L8" s="0"/>
-    </row>
-    <row r="9" customFormat="false" ht="49.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="L8" s="10"/>
+    </row>
+    <row r="9" s="13" customFormat="true" ht="49.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="0" t="s">
+      <c r="E9" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="G9" s="0"/>
-      <c r="H9" s="2" t="s">
+      <c r="G9" s="10"/>
+      <c r="H9" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="I9" s="3" t="s">
+      <c r="I9" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="L9" s="13" t="s">
+      <c r="L9" s="14" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="55.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+    <row r="10" s="13" customFormat="true" ht="55.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="E10" s="0" t="s">
+      <c r="E10" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="F10" s="0" t="s">
+      <c r="F10" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="G10" s="0"/>
-      <c r="H10" s="2" t="s">
+      <c r="G10" s="10"/>
+      <c r="H10" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="I10" s="3" t="s">
+      <c r="I10" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="L10" s="13" t="s">
+      <c r="L10" s="14" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1636,10 +1636,10 @@
       <c r="D11" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="E11" s="14" t="s">
+      <c r="E11" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="F11" s="14"/>
+      <c r="F11" s="15"/>
       <c r="H11" s="10" t="s">
         <v>26</v>
       </c>
@@ -1689,10 +1689,10 @@
       <c r="D13" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E13" s="15" t="s">
+      <c r="E13" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="F13" s="15"/>
+      <c r="F13" s="16"/>
       <c r="G13" s="0"/>
       <c r="H13" s="2" t="s">
         <v>26</v>
@@ -1718,7 +1718,7 @@
       <c r="E14" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="F14" s="16"/>
+      <c r="F14" s="10"/>
       <c r="G14" s="17" t="s">
         <v>53</v>
       </c>
@@ -1746,7 +1746,7 @@
       <c r="E15" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="F15" s="16"/>
+      <c r="F15" s="10"/>
       <c r="G15" s="17" t="s">
         <v>56</v>
       </c>
@@ -1758,7 +1758,7 @@
       </c>
       <c r="L15" s="0"/>
     </row>
-    <row r="16" s="16" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="16" s="10" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="10" t="s">
         <v>21</v>
       </c>
@@ -1787,83 +1787,83 @@
         <v>60</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+    <row r="17" s="13" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="0" t="s">
+      <c r="B17" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C17" s="0" t="s">
+      <c r="C17" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="E17" s="0" t="s">
+      <c r="E17" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="G17" s="0"/>
-      <c r="H17" s="2" t="s">
+      <c r="G17" s="10"/>
+      <c r="H17" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="I17" s="3" t="s">
+      <c r="I17" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="L17" s="0"/>
-    </row>
-    <row r="18" customFormat="false" ht="43.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="L17" s="10"/>
+    </row>
+    <row r="18" s="13" customFormat="true" ht="43.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="B18" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="0" t="s">
+      <c r="C18" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="E18" s="0" t="s">
+      <c r="E18" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="F18" s="0" t="s">
+      <c r="F18" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="G18" s="0"/>
-      <c r="H18" s="2" t="s">
+      <c r="G18" s="10"/>
+      <c r="H18" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="I18" s="3" t="s">
+      <c r="I18" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="L18" s="0"/>
-    </row>
-    <row r="19" customFormat="false" ht="38.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="L18" s="10"/>
+    </row>
+    <row r="19" s="13" customFormat="true" ht="38.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="B19" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="0" t="s">
+      <c r="C19" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D19" s="11" t="s">
         <v>24</v>
       </c>
       <c r="E19" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="G19" s="0"/>
-      <c r="H19" s="2" t="s">
+      <c r="G19" s="10"/>
+      <c r="H19" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="I19" s="3" t="s">
+      <c r="I19" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="L19" s="0"/>
+      <c r="L19" s="10"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
@@ -1999,7 +1999,7 @@
       <c r="D25" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="E25" s="22" t="s">
+      <c r="E25" s="19" t="s">
         <v>80</v>
       </c>
       <c r="F25" s="10" t="s">
@@ -2020,7 +2020,7 @@
       <c r="D26" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="E26" s="22" t="s">
+      <c r="E26" s="19" t="s">
         <v>80</v>
       </c>
       <c r="G26" s="10"/>
@@ -2032,85 +2032,85 @@
       </c>
       <c r="L26" s="12"/>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
+    <row r="27" s="13" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="B27" s="0" t="s">
+      <c r="B27" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="C27" s="0" t="s">
+      <c r="C27" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="D27" s="11" t="s">
         <v>79</v>
       </c>
       <c r="E27" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="G27" s="0"/>
-      <c r="H27" s="0"/>
-      <c r="I27" s="0"/>
-    </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
+      <c r="G27" s="10"/>
+      <c r="H27" s="10"/>
+      <c r="I27" s="10"/>
+    </row>
+    <row r="28" s="13" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="B28" s="0" t="s">
+      <c r="B28" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="C28" s="0" t="s">
+      <c r="C28" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="D28" s="11" t="s">
         <v>79</v>
       </c>
       <c r="E28" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="G28" s="0"/>
-      <c r="H28" s="0"/>
-      <c r="I28" s="0"/>
-    </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
+      <c r="G28" s="10"/>
+      <c r="H28" s="10"/>
+      <c r="I28" s="10"/>
+    </row>
+    <row r="29" s="13" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A29" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="B29" s="0" t="s">
+      <c r="B29" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="C29" s="0" t="s">
+      <c r="C29" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="D29" s="11" t="s">
         <v>79</v>
       </c>
       <c r="E29" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="G29" s="0"/>
-      <c r="H29" s="0"/>
-      <c r="I29" s="0"/>
-    </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
+      <c r="G29" s="10"/>
+      <c r="H29" s="10"/>
+      <c r="I29" s="10"/>
+    </row>
+    <row r="30" s="13" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A30" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="B30" s="0" t="s">
+      <c r="B30" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="C30" s="0" t="s">
+      <c r="C30" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="D30" s="11" t="s">
         <v>79</v>
       </c>
       <c r="E30" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="G30" s="0"/>
-      <c r="H30" s="0"/>
-      <c r="I30" s="0"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="10"/>
+      <c r="I30" s="10"/>
     </row>
     <row r="31" s="10" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="10" t="s">
@@ -2125,131 +2125,130 @@
       <c r="D31" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="E31" s="14" t="s">
+      <c r="E31" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="F31" s="16"/>
       <c r="L31" s="12"/>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
+    <row r="32" s="13" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A32" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="B32" s="0" t="s">
+      <c r="B32" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="C32" s="0" t="s">
+      <c r="C32" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="D32" s="11" t="s">
         <v>79</v>
       </c>
       <c r="E32" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="G32" s="0"/>
-      <c r="H32" s="0"/>
-      <c r="I32" s="0"/>
-    </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
+      <c r="G32" s="10"/>
+      <c r="H32" s="10"/>
+      <c r="I32" s="10"/>
+    </row>
+    <row r="33" s="13" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A33" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="B33" s="0" t="s">
+      <c r="B33" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="C33" s="0" t="s">
+      <c r="C33" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="D33" s="11" t="s">
         <v>79</v>
       </c>
       <c r="E33" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="G33" s="0"/>
-      <c r="H33" s="0"/>
-      <c r="I33" s="0"/>
-    </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
+      <c r="G33" s="10"/>
+      <c r="H33" s="10"/>
+      <c r="I33" s="10"/>
+    </row>
+    <row r="34" s="13" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A34" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="B34" s="0" t="s">
+      <c r="B34" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="C34" s="0" t="s">
+      <c r="C34" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="D34" s="11" t="s">
         <v>79</v>
       </c>
       <c r="E34" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="G34" s="0"/>
-      <c r="H34" s="0"/>
-      <c r="I34" s="0"/>
-    </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
+      <c r="G34" s="10"/>
+      <c r="H34" s="10"/>
+      <c r="I34" s="10"/>
+    </row>
+    <row r="35" s="13" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A35" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="B35" s="0" t="s">
+      <c r="B35" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="C35" s="0" t="s">
+      <c r="C35" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="D35" s="11" t="s">
         <v>79</v>
       </c>
       <c r="E35" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="G35" s="0"/>
-      <c r="H35" s="0"/>
-      <c r="I35" s="0"/>
-    </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
+      <c r="G35" s="10"/>
+      <c r="H35" s="10"/>
+      <c r="I35" s="10"/>
+    </row>
+    <row r="36" s="13" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A36" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="B36" s="0" t="s">
+      <c r="B36" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="C36" s="0" t="s">
+      <c r="C36" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="D36" s="11" t="s">
         <v>79</v>
       </c>
       <c r="E36" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="G36" s="0"/>
-      <c r="H36" s="0"/>
-      <c r="I36" s="0"/>
-    </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
+      <c r="G36" s="10"/>
+      <c r="H36" s="10"/>
+      <c r="I36" s="10"/>
+    </row>
+    <row r="37" s="13" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A37" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="B37" s="0" t="s">
+      <c r="B37" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="C37" s="0" t="s">
+      <c r="C37" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="D37" s="1" t="s">
+      <c r="D37" s="11" t="s">
         <v>79</v>
       </c>
       <c r="E37" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="G37" s="0"/>
-      <c r="H37" s="0"/>
-      <c r="I37" s="0"/>
+      <c r="G37" s="10"/>
+      <c r="H37" s="10"/>
+      <c r="I37" s="10"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="10" t="s">
@@ -2267,7 +2266,7 @@
       <c r="E38" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="F38" s="16"/>
+      <c r="F38" s="10"/>
       <c r="G38" s="17" t="s">
         <v>53</v>
       </c>
@@ -2277,6 +2276,7 @@
       <c r="I38" s="11" t="s">
         <v>54</v>
       </c>
+      <c r="L38" s="0"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="10" t="s">
@@ -2294,7 +2294,7 @@
       <c r="E39" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="F39" s="16"/>
+      <c r="F39" s="10"/>
       <c r="G39" s="17" t="s">
         <v>56</v>
       </c>
@@ -2304,6 +2304,7 @@
       <c r="I39" s="11" t="s">
         <v>57</v>
       </c>
+      <c r="L39" s="0"/>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="10" t="s">
@@ -2333,55 +2334,56 @@
       <c r="I40" s="11" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="s">
+      <c r="L40" s="0"/>
+    </row>
+    <row r="41" s="13" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A41" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="B41" s="0" t="s">
+      <c r="B41" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="C41" s="0" t="s">
+      <c r="C41" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="D41" s="1" t="s">
+      <c r="D41" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="E41" s="0" t="s">
+      <c r="E41" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="G41" s="0"/>
-      <c r="H41" s="2" t="s">
+      <c r="G41" s="10"/>
+      <c r="H41" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="I41" s="3" t="s">
+      <c r="I41" s="11" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="s">
+    <row r="42" s="13" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A42" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="B42" s="0" t="s">
+      <c r="B42" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="C42" s="0" t="s">
+      <c r="C42" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="D42" s="1" t="s">
+      <c r="D42" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="E42" s="0" t="s">
+      <c r="E42" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="F42" s="0" t="s">
+      <c r="F42" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="G42" s="0"/>
-      <c r="H42" s="2" t="s">
+      <c r="G42" s="10"/>
+      <c r="H42" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="I42" s="3" t="s">
+      <c r="I42" s="11" t="s">
         <v>63</v>
       </c>
     </row>
@@ -2398,10 +2400,9 @@
       <c r="D43" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="E43" s="22" t="s">
+      <c r="E43" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="F43" s="16"/>
       <c r="H43" s="10" t="s">
         <v>26</v>
       </c>
@@ -2438,6 +2439,7 @@
       <c r="I44" s="3" t="s">
         <v>68</v>
       </c>
+      <c r="L44" s="0"/>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
@@ -2465,6 +2467,7 @@
       <c r="I45" s="3" t="s">
         <v>70</v>
       </c>
+      <c r="L45" s="0"/>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
@@ -2491,6 +2494,7 @@
       <c r="I46" s="21" t="s">
         <v>71</v>
       </c>
+      <c r="L46" s="0"/>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="10" t="s">
@@ -2520,11 +2524,13 @@
       <c r="I47" s="11" t="s">
         <v>75</v>
       </c>
+      <c r="L47" s="0"/>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="G48" s="0"/>
       <c r="H48" s="0"/>
       <c r="I48" s="0"/>
+      <c r="L48" s="0"/>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="10" t="s">
@@ -2542,7 +2548,7 @@
       <c r="E49" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="F49" s="16"/>
+      <c r="F49" s="10"/>
       <c r="G49" s="10"/>
       <c r="H49" s="10" t="s">
         <v>26</v>
@@ -2550,326 +2556,327 @@
       <c r="I49" s="11" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A50" s="0" t="s">
+      <c r="L49" s="0"/>
+    </row>
+    <row r="50" s="13" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A50" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="B50" s="0" t="s">
+      <c r="B50" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="C50" s="0" t="s">
+      <c r="C50" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="D50" s="1" t="s">
+      <c r="D50" s="11" t="s">
         <v>103</v>
       </c>
       <c r="E50" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="G50" s="0"/>
-      <c r="H50" s="0"/>
-      <c r="I50" s="0"/>
-    </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A51" s="0" t="s">
+      <c r="G50" s="10"/>
+      <c r="H50" s="10"/>
+      <c r="I50" s="10"/>
+    </row>
+    <row r="51" s="13" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A51" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="B51" s="0" t="s">
+      <c r="B51" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="C51" s="0" t="s">
+      <c r="C51" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="D51" s="1" t="s">
+      <c r="D51" s="11" t="s">
         <v>103</v>
       </c>
       <c r="E51" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="G51" s="0"/>
-      <c r="H51" s="0"/>
-      <c r="I51" s="0"/>
-    </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0" t="s">
+      <c r="G51" s="10"/>
+      <c r="H51" s="10"/>
+      <c r="I51" s="10"/>
+    </row>
+    <row r="52" s="13" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A52" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="B52" s="0" t="s">
+      <c r="B52" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="C52" s="0" t="s">
+      <c r="C52" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="D52" s="1" t="s">
+      <c r="D52" s="11" t="s">
         <v>103</v>
       </c>
       <c r="E52" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="G52" s="0"/>
-      <c r="H52" s="0"/>
-      <c r="I52" s="0"/>
-    </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0" t="s">
+      <c r="G52" s="10"/>
+      <c r="H52" s="10"/>
+      <c r="I52" s="10"/>
+    </row>
+    <row r="53" s="13" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A53" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="B53" s="0" t="s">
+      <c r="B53" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="C53" s="0" t="s">
+      <c r="C53" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="D53" s="1" t="s">
+      <c r="D53" s="11" t="s">
         <v>103</v>
       </c>
       <c r="E53" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="G53" s="0"/>
-      <c r="H53" s="0"/>
-      <c r="I53" s="0"/>
-    </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A54" s="0" t="s">
+      <c r="G53" s="10"/>
+      <c r="H53" s="10"/>
+      <c r="I53" s="10"/>
+    </row>
+    <row r="54" s="13" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A54" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="B54" s="0" t="s">
+      <c r="B54" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="C54" s="0" t="s">
+      <c r="C54" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="D54" s="1" t="s">
+      <c r="D54" s="11" t="s">
         <v>103</v>
       </c>
       <c r="E54" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="G54" s="0"/>
-      <c r="H54" s="0"/>
-      <c r="I54" s="0"/>
-    </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A55" s="0" t="s">
+      <c r="G54" s="10"/>
+      <c r="H54" s="10"/>
+      <c r="I54" s="10"/>
+    </row>
+    <row r="55" s="13" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A55" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="B55" s="0" t="s">
+      <c r="B55" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="C55" s="0" t="s">
+      <c r="C55" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="D55" s="1" t="s">
+      <c r="D55" s="11" t="s">
         <v>103</v>
       </c>
       <c r="E55" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="G55" s="0"/>
-      <c r="H55" s="0"/>
-      <c r="I55" s="0"/>
-    </row>
-    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A56" s="0" t="s">
+      <c r="G55" s="10"/>
+      <c r="H55" s="10"/>
+      <c r="I55" s="10"/>
+    </row>
+    <row r="56" s="13" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A56" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="B56" s="0" t="s">
+      <c r="B56" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="C56" s="0" t="s">
+      <c r="C56" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="D56" s="1" t="s">
+      <c r="D56" s="11" t="s">
         <v>103</v>
       </c>
       <c r="E56" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="G56" s="0"/>
-      <c r="H56" s="0"/>
-      <c r="I56" s="0"/>
-    </row>
-    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A57" s="0" t="s">
+      <c r="G56" s="10"/>
+      <c r="H56" s="10"/>
+      <c r="I56" s="10"/>
+    </row>
+    <row r="57" s="13" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A57" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="B57" s="0" t="s">
+      <c r="B57" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="C57" s="0" t="s">
+      <c r="C57" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="D57" s="1" t="s">
+      <c r="D57" s="11" t="s">
         <v>103</v>
       </c>
       <c r="E57" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="G57" s="0"/>
-      <c r="H57" s="0"/>
-      <c r="I57" s="0"/>
-    </row>
-    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A58" s="0" t="s">
+      <c r="G57" s="10"/>
+      <c r="H57" s="10"/>
+      <c r="I57" s="10"/>
+    </row>
+    <row r="58" s="13" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A58" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="B58" s="0" t="s">
+      <c r="B58" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="C58" s="0" t="s">
+      <c r="C58" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="D58" s="1" t="s">
+      <c r="D58" s="11" t="s">
         <v>103</v>
       </c>
       <c r="E58" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="G58" s="0"/>
-      <c r="H58" s="0"/>
-      <c r="I58" s="0"/>
-    </row>
-    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A59" s="0" t="s">
+      <c r="G58" s="10"/>
+      <c r="H58" s="10"/>
+      <c r="I58" s="10"/>
+    </row>
+    <row r="59" s="13" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A59" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="B59" s="0" t="s">
+      <c r="B59" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="C59" s="0" t="s">
+      <c r="C59" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="D59" s="1" t="s">
+      <c r="D59" s="11" t="s">
         <v>103</v>
       </c>
       <c r="E59" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="G59" s="0"/>
-      <c r="H59" s="0"/>
-      <c r="I59" s="0"/>
-    </row>
-    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A60" s="0" t="s">
+      <c r="G59" s="10"/>
+      <c r="H59" s="10"/>
+      <c r="I59" s="10"/>
+    </row>
+    <row r="60" s="13" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A60" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="B60" s="0" t="s">
+      <c r="B60" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="C60" s="0" t="s">
+      <c r="C60" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="D60" s="1" t="s">
+      <c r="D60" s="11" t="s">
         <v>103</v>
       </c>
       <c r="E60" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="G60" s="0"/>
-      <c r="H60" s="0"/>
-      <c r="I60" s="0"/>
-    </row>
-    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A61" s="0" t="s">
+      <c r="G60" s="10"/>
+      <c r="H60" s="10"/>
+      <c r="I60" s="10"/>
+    </row>
+    <row r="61" s="13" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A61" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="B61" s="0" t="s">
+      <c r="B61" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="C61" s="0" t="s">
+      <c r="C61" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="D61" s="1" t="s">
+      <c r="D61" s="11" t="s">
         <v>103</v>
       </c>
       <c r="E61" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="G61" s="0"/>
-      <c r="H61" s="0"/>
-      <c r="I61" s="0"/>
-    </row>
-    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A62" s="0" t="s">
+      <c r="G61" s="10"/>
+      <c r="H61" s="10"/>
+      <c r="I61" s="10"/>
+    </row>
+    <row r="62" s="13" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A62" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="B62" s="0" t="s">
+      <c r="B62" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="C62" s="0" t="s">
+      <c r="C62" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="D62" s="1" t="s">
+      <c r="D62" s="11" t="s">
         <v>103</v>
       </c>
       <c r="E62" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="G62" s="0"/>
-      <c r="H62" s="0"/>
-      <c r="I62" s="0"/>
-    </row>
-    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A63" s="0" t="s">
+      <c r="G62" s="10"/>
+      <c r="H62" s="10"/>
+      <c r="I62" s="10"/>
+    </row>
+    <row r="63" s="13" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A63" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="B63" s="0" t="s">
+      <c r="B63" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="C63" s="0" t="s">
+      <c r="C63" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="D63" s="1" t="s">
+      <c r="D63" s="11" t="s">
         <v>103</v>
       </c>
       <c r="E63" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="G63" s="0"/>
-      <c r="H63" s="0"/>
-      <c r="I63" s="0"/>
-    </row>
-    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A64" s="0" t="s">
+      <c r="G63" s="10"/>
+      <c r="H63" s="10"/>
+      <c r="I63" s="10"/>
+    </row>
+    <row r="64" s="13" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A64" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="B64" s="0" t="s">
+      <c r="B64" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="C64" s="0" t="s">
+      <c r="C64" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="D64" s="1" t="s">
+      <c r="D64" s="11" t="s">
         <v>103</v>
       </c>
       <c r="E64" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="G64" s="0"/>
-      <c r="H64" s="0"/>
-      <c r="I64" s="0"/>
-    </row>
-    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A65" s="0" t="s">
+      <c r="G64" s="10"/>
+      <c r="H64" s="10"/>
+      <c r="I64" s="10"/>
+    </row>
+    <row r="65" s="13" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A65" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="B65" s="0" t="s">
+      <c r="B65" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="C65" s="0" t="s">
+      <c r="C65" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="D65" s="1" t="s">
+      <c r="D65" s="11" t="s">
         <v>103</v>
       </c>
       <c r="E65" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="G65" s="0"/>
-      <c r="H65" s="0"/>
-      <c r="I65" s="0"/>
+      <c r="G65" s="10"/>
+      <c r="H65" s="10"/>
+      <c r="I65" s="10"/>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
@@ -2896,6 +2903,7 @@
       <c r="I66" s="3" t="s">
         <v>54</v>
       </c>
+      <c r="L66" s="0"/>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
@@ -2922,6 +2930,7 @@
       <c r="I67" s="3" t="s">
         <v>57</v>
       </c>
+      <c r="L67" s="0"/>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
@@ -2942,7 +2951,7 @@
       <c r="F68" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="G68" s="23" t="s">
+      <c r="G68" s="22" t="s">
         <v>122</v>
       </c>
       <c r="H68" s="2" t="s">
@@ -2951,55 +2960,56 @@
       <c r="I68" s="3" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A69" s="0" t="s">
+      <c r="L68" s="0"/>
+    </row>
+    <row r="69" s="13" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A69" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="B69" s="0" t="s">
+      <c r="B69" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="C69" s="0" t="s">
+      <c r="C69" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="D69" s="1" t="s">
+      <c r="D69" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="E69" s="0" t="s">
+      <c r="E69" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="G69" s="0"/>
-      <c r="H69" s="2" t="s">
+      <c r="G69" s="10"/>
+      <c r="H69" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="I69" s="3" t="s">
+      <c r="I69" s="11" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A70" s="0" t="s">
+    <row r="70" s="13" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A70" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="B70" s="0" t="s">
+      <c r="B70" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="C70" s="0" t="s">
+      <c r="C70" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="D70" s="1" t="s">
+      <c r="D70" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="E70" s="0" t="s">
+      <c r="E70" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="F70" s="0" t="s">
+      <c r="F70" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="G70" s="0"/>
-      <c r="H70" s="2" t="s">
+      <c r="G70" s="10"/>
+      <c r="H70" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="I70" s="3" t="s">
+      <c r="I70" s="11" t="s">
         <v>63</v>
       </c>
     </row>
@@ -3016,10 +3026,9 @@
       <c r="D71" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="E71" s="22" t="s">
+      <c r="E71" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="F71" s="16"/>
       <c r="H71" s="10" t="s">
         <v>26</v>
       </c>
@@ -3110,34 +3119,35 @@
         <v>71</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A75" s="0" t="s">
+    <row r="75" s="10" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A75" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="B75" s="0" t="s">
+      <c r="B75" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="C75" s="0" t="s">
+      <c r="C75" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="D75" s="1" t="s">
+      <c r="D75" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="E75" s="0" t="s">
+      <c r="E75" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="F75" s="0" t="s">
+      <c r="F75" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="G75" s="21" t="s">
+      <c r="G75" s="23" t="s">
         <v>101</v>
       </c>
-      <c r="H75" s="2" t="s">
+      <c r="H75" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="I75" s="3" t="s">
+      <c r="I75" s="11" t="s">
         <v>75</v>
       </c>
+      <c r="L75" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
[ issue #8 ] DC Mapping file
</commit_message>
<xml_diff>
--- a/aliada/src/site/analysis/mapping_dctordf_v1.1.xlsx
+++ b/aliada/src/site/analysis/mapping_dctordf_v1.1.xlsx
@@ -1116,7 +1116,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1133,12 +1133,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFDDD9C3"/>
         <bgColor rgb="FFFFCC99"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00CC33"/>
-        <bgColor rgb="FF339966"/>
       </patternFill>
     </fill>
   </fills>
@@ -1193,7 +1187,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1234,43 +1228,27 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="4" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1278,15 +1256,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1305,7 +1283,7 @@
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
       <rgbColor rgb="FFFF0000"/>
-      <rgbColor rgb="FF00CC33"/>
+      <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
@@ -1368,10 +1346,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L75"/>
+  <dimension ref="A1:L76"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I21" activeCellId="0" sqref="I21"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A18" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A91" activeCellId="0" sqref="6:91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1511,7 +1489,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="7" s="13" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="10" t="s">
         <v>21</v>
       </c>
@@ -1648,61 +1626,57 @@
       </c>
       <c r="L11" s="12"/>
     </row>
-    <row r="12" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+    <row r="12" s="13" customFormat="true" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="C12" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="E12" s="0" t="s">
+      <c r="E12" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="F12" s="0" t="s">
+      <c r="F12" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="G12" s="0"/>
-      <c r="H12" s="2" t="s">
+      <c r="H12" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="I12" s="3" t="s">
+      <c r="I12" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="L12" s="0"/>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+    </row>
+    <row r="13" s="13" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="C13" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="E13" s="16" t="s">
+      <c r="E13" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="F13" s="16"/>
-      <c r="G13" s="0"/>
-      <c r="H13" s="2" t="s">
+      <c r="F13" s="15"/>
+      <c r="H13" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="I13" s="3" t="s">
+      <c r="I13" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="L13" s="0"/>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="14" s="13" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="10" t="s">
         <v>21</v>
       </c>
@@ -1719,7 +1693,7 @@
         <v>52</v>
       </c>
       <c r="F14" s="10"/>
-      <c r="G14" s="17" t="s">
+      <c r="G14" s="16" t="s">
         <v>53</v>
       </c>
       <c r="H14" s="10" t="s">
@@ -1728,9 +1702,8 @@
       <c r="I14" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="L14" s="0"/>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="15" s="13" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="10" t="s">
         <v>21</v>
       </c>
@@ -1747,7 +1720,7 @@
         <v>55</v>
       </c>
       <c r="F15" s="10"/>
-      <c r="G15" s="17" t="s">
+      <c r="G15" s="16" t="s">
         <v>56</v>
       </c>
       <c r="H15" s="10" t="s">
@@ -1756,7 +1729,6 @@
       <c r="I15" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="L15" s="0"/>
     </row>
     <row r="16" s="10" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="10" t="s">
@@ -1777,7 +1749,7 @@
       <c r="F16" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="G16" s="18" t="s">
+      <c r="G16" s="17" t="s">
         <v>59</v>
       </c>
       <c r="H16" s="10" t="s">
@@ -1853,7 +1825,7 @@
       <c r="D19" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="E19" s="19" t="s">
+      <c r="E19" s="18" t="s">
         <v>64</v>
       </c>
       <c r="G19" s="10"/>
@@ -1865,92 +1837,88 @@
       </c>
       <c r="L19" s="10"/>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+    <row r="20" s="13" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="0" t="s">
+      <c r="B20" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="C20" s="0" t="s">
+      <c r="C20" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D20" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="E20" s="0" t="s">
+      <c r="E20" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="F20" s="0" t="s">
+      <c r="F20" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="G20" s="20" t="s">
+      <c r="G20" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="H20" s="2" t="s">
+      <c r="H20" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="I20" s="3" t="s">
+      <c r="I20" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="L20" s="0"/>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+    </row>
+    <row r="21" s="13" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="B21" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="C21" s="0" t="s">
+      <c r="C21" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D21" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="E21" s="0" t="s">
+      <c r="E21" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="F21" s="0" t="s">
+      <c r="F21" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="G21" s="0"/>
-      <c r="H21" s="2" t="s">
+      <c r="H21" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="I21" s="3" t="s">
+      <c r="I21" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="L21" s="0"/>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+    </row>
+    <row r="22" s="13" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="0" t="s">
+      <c r="B22" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="0" t="s">
+      <c r="C22" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D22" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="E22" s="0" t="s">
+      <c r="E22" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="G22" s="20" t="s">
+      <c r="G22" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="H22" s="2" t="s">
+      <c r="H22" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="I22" s="21" t="s">
+      <c r="I22" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="L22" s="0"/>
-    </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="23" s="13" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="10" t="s">
         <v>21</v>
       </c>
@@ -1969,7 +1937,7 @@
       <c r="F23" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="G23" s="17" t="s">
+      <c r="G23" s="16" t="s">
         <v>74</v>
       </c>
       <c r="H23" s="10" t="s">
@@ -1978,14 +1946,8 @@
       <c r="I23" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="L23" s="0"/>
-    </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G24" s="0"/>
-      <c r="H24" s="0"/>
-      <c r="I24" s="0"/>
-      <c r="L24" s="0"/>
-    </row>
+    </row>
+    <row r="24" s="13" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="25" s="10" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="10" t="s">
         <v>76</v>
@@ -1999,7 +1961,7 @@
       <c r="D25" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="E25" s="19" t="s">
+      <c r="E25" s="18" t="s">
         <v>80</v>
       </c>
       <c r="F25" s="10" t="s">
@@ -2007,7 +1969,7 @@
       </c>
       <c r="L25" s="12"/>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="26" s="13" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="10" t="s">
         <v>76</v>
       </c>
@@ -2020,7 +1982,7 @@
       <c r="D26" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="E26" s="19" t="s">
+      <c r="E26" s="18" t="s">
         <v>80</v>
       </c>
       <c r="G26" s="10"/>
@@ -2163,7 +2125,7 @@
       <c r="D33" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="E33" s="19" t="s">
+      <c r="E33" s="18" t="s">
         <v>92</v>
       </c>
       <c r="G33" s="10"/>
@@ -2203,7 +2165,7 @@
       <c r="D35" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="E35" s="19" t="s">
+      <c r="E35" s="18" t="s">
         <v>32</v>
       </c>
       <c r="G35" s="10"/>
@@ -2250,7 +2212,7 @@
       <c r="H37" s="10"/>
       <c r="I37" s="10"/>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="38" s="13" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="10" t="s">
         <v>76</v>
       </c>
@@ -2267,7 +2229,7 @@
         <v>52</v>
       </c>
       <c r="F38" s="10"/>
-      <c r="G38" s="17" t="s">
+      <c r="G38" s="16" t="s">
         <v>53</v>
       </c>
       <c r="H38" s="10" t="s">
@@ -2276,9 +2238,8 @@
       <c r="I38" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="L38" s="0"/>
-    </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="39" s="13" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="10" t="s">
         <v>76</v>
       </c>
@@ -2295,7 +2256,7 @@
         <v>55</v>
       </c>
       <c r="F39" s="10"/>
-      <c r="G39" s="17" t="s">
+      <c r="G39" s="16" t="s">
         <v>56</v>
       </c>
       <c r="H39" s="10" t="s">
@@ -2304,9 +2265,8 @@
       <c r="I39" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="L39" s="0"/>
-    </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="40" s="13" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="10" t="s">
         <v>76</v>
       </c>
@@ -2325,7 +2285,7 @@
       <c r="F40" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="G40" s="18" t="s">
+      <c r="G40" s="17" t="s">
         <v>98</v>
       </c>
       <c r="H40" s="10" t="s">
@@ -2334,7 +2294,6 @@
       <c r="I40" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="L40" s="0"/>
     </row>
     <row r="41" s="13" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="10" t="s">
@@ -2400,7 +2359,7 @@
       <c r="D43" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="E43" s="19" t="s">
+      <c r="E43" s="18" t="s">
         <v>64</v>
       </c>
       <c r="H43" s="10" t="s">
@@ -2411,92 +2370,88 @@
       </c>
       <c r="L43" s="12"/>
     </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="s">
+    <row r="44" s="13" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A44" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="B44" s="0" t="s">
+      <c r="B44" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="C44" s="0" t="s">
+      <c r="C44" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="D44" s="1" t="s">
+      <c r="D44" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="E44" s="0" t="s">
+      <c r="E44" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="F44" s="0" t="s">
+      <c r="F44" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="G44" s="20" t="s">
+      <c r="G44" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="H44" s="2" t="s">
+      <c r="H44" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="I44" s="3" t="s">
+      <c r="I44" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="L44" s="0"/>
-    </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
+    </row>
+    <row r="45" s="13" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A45" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="B45" s="0" t="s">
+      <c r="B45" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="C45" s="0" t="s">
+      <c r="C45" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="D45" s="1" t="s">
+      <c r="D45" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="E45" s="0" t="s">
+      <c r="E45" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="F45" s="0" t="s">
+      <c r="F45" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="G45" s="0"/>
-      <c r="H45" s="2" t="s">
+      <c r="H45" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="I45" s="3" t="s">
+      <c r="I45" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="L45" s="0"/>
-    </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
+    </row>
+    <row r="46" s="13" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A46" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="B46" s="0" t="s">
+      <c r="B46" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="C46" s="0" t="s">
+      <c r="C46" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="D46" s="1" t="s">
+      <c r="D46" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="E46" s="0" t="s">
+      <c r="E46" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="G46" s="20" t="s">
+      <c r="G46" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="H46" s="2" t="s">
+      <c r="H46" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="I46" s="21" t="s">
+      <c r="I46" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="L46" s="0"/>
-    </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="47" s="13" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="10" t="s">
         <v>76</v>
       </c>
@@ -2515,7 +2470,7 @@
       <c r="F47" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="G47" s="17" t="s">
+      <c r="G47" s="16" t="s">
         <v>100</v>
       </c>
       <c r="H47" s="10" t="s">
@@ -2524,15 +2479,9 @@
       <c r="I47" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="L47" s="0"/>
-    </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G48" s="0"/>
-      <c r="H48" s="0"/>
-      <c r="I48" s="0"/>
-      <c r="L48" s="0"/>
-    </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="48" s="13" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="49" s="13" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="10" t="s">
         <v>101</v>
       </c>
@@ -2556,7 +2505,6 @@
       <c r="I49" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="L49" s="0"/>
     </row>
     <row r="50" s="13" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="10" t="s">
@@ -2878,89 +2826,86 @@
       <c r="H65" s="10"/>
       <c r="I65" s="10"/>
     </row>
-    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A66" s="0" t="s">
+    <row r="66" s="13" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A66" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="B66" s="0" t="s">
+      <c r="B66" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="C66" s="0" t="s">
+      <c r="C66" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="D66" s="1" t="s">
+      <c r="D66" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="E66" s="0" t="s">
+      <c r="E66" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="G66" s="20" t="s">
+      <c r="G66" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="H66" s="2" t="s">
+      <c r="H66" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="I66" s="3" t="s">
+      <c r="I66" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="L66" s="0"/>
-    </row>
-    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A67" s="0" t="s">
+    </row>
+    <row r="67" s="13" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A67" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="B67" s="0" t="s">
+      <c r="B67" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="C67" s="0" t="s">
+      <c r="C67" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="D67" s="1" t="s">
+      <c r="D67" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="E67" s="0" t="s">
+      <c r="E67" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="G67" s="20" t="s">
+      <c r="G67" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="H67" s="2" t="s">
+      <c r="H67" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="I67" s="3" t="s">
+      <c r="I67" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="L67" s="0"/>
-    </row>
-    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A68" s="0" t="s">
+    </row>
+    <row r="68" s="13" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A68" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="B68" s="0" t="s">
+      <c r="B68" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="C68" s="0" t="s">
+      <c r="C68" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="D68" s="1" t="s">
+      <c r="D68" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="E68" s="0" t="s">
+      <c r="E68" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="F68" s="0" t="s">
+      <c r="F68" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="G68" s="22" t="s">
+      <c r="G68" s="17" t="s">
         <v>122</v>
       </c>
-      <c r="H68" s="2" t="s">
+      <c r="H68" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="I68" s="3" t="s">
+      <c r="I68" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="L68" s="0"/>
     </row>
     <row r="69" s="13" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="10" t="s">
@@ -3026,7 +2971,7 @@
       <c r="D71" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="E71" s="19" t="s">
+      <c r="E71" s="18" t="s">
         <v>64</v>
       </c>
       <c r="H71" s="10" t="s">
@@ -3037,85 +2982,84 @@
       </c>
       <c r="L71" s="12"/>
     </row>
-    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A72" s="0" t="s">
+    <row r="72" s="13" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A72" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="B72" s="0" t="s">
+      <c r="B72" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="C72" s="0" t="s">
+      <c r="C72" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="D72" s="1" t="s">
+      <c r="D72" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="E72" s="0" t="s">
+      <c r="E72" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="F72" s="0" t="s">
+      <c r="F72" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="G72" s="20" t="s">
+      <c r="G72" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="H72" s="2" t="s">
+      <c r="H72" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="I72" s="3" t="s">
+      <c r="I72" s="11" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A73" s="0" t="s">
+    <row r="73" s="13" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A73" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="B73" s="0" t="s">
+      <c r="B73" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="C73" s="0" t="s">
+      <c r="C73" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="D73" s="1" t="s">
+      <c r="D73" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="E73" s="0" t="s">
+      <c r="E73" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="F73" s="0" t="s">
+      <c r="F73" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="G73" s="0"/>
-      <c r="H73" s="2" t="s">
+      <c r="H73" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="I73" s="3" t="s">
+      <c r="I73" s="11" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A74" s="0" t="s">
+    <row r="74" s="13" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A74" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="B74" s="0" t="s">
+      <c r="B74" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="C74" s="0" t="s">
+      <c r="C74" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="D74" s="1" t="s">
+      <c r="D74" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="E74" s="0" t="s">
+      <c r="E74" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="G74" s="20" t="s">
+      <c r="G74" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="H74" s="2" t="s">
+      <c r="H74" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="I74" s="21" t="s">
+      <c r="I74" s="19" t="s">
         <v>71</v>
       </c>
     </row>
@@ -3138,7 +3082,7 @@
       <c r="F75" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="G75" s="23" t="s">
+      <c r="G75" s="19" t="s">
         <v>101</v>
       </c>
       <c r="H75" s="10" t="s">
@@ -3149,6 +3093,22 @@
       </c>
       <c r="L75" s="12"/>
     </row>
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="E1:I2"/>

</xml_diff>